<commit_message>
change color evaluation proccess add draw boreholes functions
</commit_message>
<xml_diff>
--- a/tests/data/t_borehole2D.xlsx
+++ b/tests/data/t_borehole2D.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\papau\Desktop\Projetospessoais\geotechnics\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24148D86-B601-4DD8-841E-EC6228A69CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA7FF67-B84D-420D-BADA-772153209621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="945" windowWidth="29040" windowHeight="15720" xr2:uid="{9AA19384-C6D1-46CD-B2F6-04A96740206E}"/>
   </bookViews>
@@ -449,10 +449,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
add legend drawer function add docstrings to auxiliar functions fix borehole drew in wrong y direction
</commit_message>
<xml_diff>
--- a/tests/data/t_borehole2D.xlsx
+++ b/tests/data/t_borehole2D.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\papau\Desktop\Projetospessoais\geotechnics\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA7FF67-B84D-420D-BADA-772153209621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3F5240-E360-49E7-8534-E2E7AF796933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="945" windowWidth="29040" windowHeight="15720" xr2:uid="{9AA19384-C6D1-46CD-B2F6-04A96740206E}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>